<commit_message>
complete 100% shoulder and bicept both arms
</commit_message>
<xml_diff>
--- a/diagram/left_arm_diagram.xlsx
+++ b/diagram/left_arm_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Agiat_Ikazinat\Agiat_Ikazinat\diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B3D349-E84A-44FD-BF3C-326E83B15BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0038B700-F7A4-479E-BE8C-82D369A21F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1044" yWindow="2112" windowWidth="17280" windowHeight="8880" xr2:uid="{46172BA6-4082-4EE6-A904-4399B6671550}"/>
+    <workbookView xWindow="42405" yWindow="3810" windowWidth="13905" windowHeight="11235" xr2:uid="{46172BA6-4082-4EE6-A904-4399B6671550}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -83,31 +83,25 @@
     <t>Dir</t>
   </si>
   <si>
-    <t>Direction</t>
-  </si>
-  <si>
     <t>F/UP</t>
   </si>
   <si>
     <t>B/DOWN</t>
   </si>
   <si>
-    <t>F/OUT</t>
-  </si>
-  <si>
-    <t>B/IN</t>
-  </si>
-  <si>
-    <t>B/CLKW</t>
-  </si>
-  <si>
-    <t>F/CCLKW</t>
-  </si>
-  <si>
     <t>F/FONT</t>
   </si>
   <si>
     <t>B/BACK</t>
+  </si>
+  <si>
+    <t>Dir2</t>
+  </si>
+  <si>
+    <t>Inside</t>
+  </si>
+  <si>
+    <t>Outside</t>
   </si>
 </sst>
 </file>
@@ -173,7 +167,7 @@
     <tableColumn id="7" xr3:uid="{C80BBCE3-2779-4AD7-956E-DD8E4EFA71D3}" name="Dir"/>
     <tableColumn id="5" xr3:uid="{8E0D40F2-E788-4EEC-AAE3-5E8DE3741265}" name="Mid"/>
     <tableColumn id="6" xr3:uid="{A87E0A21-0844-4A09-A008-562CE01C373C}" name="Max"/>
-    <tableColumn id="9" xr3:uid="{39FC531A-BAE3-4BDB-AA25-E20517E3A0C7}" name="Direction"/>
+    <tableColumn id="9" xr3:uid="{39FC531A-BAE3-4BDB-AA25-E20517E3A0C7}" name="Dir2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -499,7 +493,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,7 +526,7 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -549,13 +543,16 @@
         <v>60</v>
       </c>
       <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>130</v>
+      </c>
+      <c r="G2">
+        <v>270</v>
+      </c>
+      <c r="H2" t="s">
         <v>21</v>
-      </c>
-      <c r="G2">
-        <v>180</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -572,16 +569,16 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F3">
-        <v>230</v>
+        <v>122</v>
       </c>
       <c r="G3">
         <v>270</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -595,16 +592,19 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>18</v>
+        <v>120</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>123</v>
       </c>
       <c r="G4">
-        <v>100</v>
+        <v>270</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -618,16 +618,19 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>124</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>35</v>
+      </c>
+      <c r="G5">
+        <v>125</v>
+      </c>
+      <c r="H5" t="s">
         <v>16</v>
-      </c>
-      <c r="G5">
-        <v>160</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>